<commit_message>
Only bill users for their first entire quarter
</commit_message>
<xml_diff>
--- a/tests/resources/mock_pi_form.xlsx
+++ b/tests/resources/mock_pi_form.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
   <si>
     <t xml:space="preserve">Timestamp</t>
   </si>
@@ -119,6 +119,18 @@
   </si>
   <si>
     <t xml:space="preserve">JJJJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kkiwi@example.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kevin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kiwi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KKKK</t>
   </si>
 </sst>
 </file>
@@ -261,13 +273,13 @@
   </sheetPr>
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="1" style="0" width="21.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="30.02"/>
@@ -436,13 +448,27 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
+      <c r="A8" s="3" t="n">
+        <v>44089.3333333333</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="3"/>
@@ -550,6 +576,7 @@
     <hyperlink ref="B5" r:id="rId4" display="ddurian@example.com"/>
     <hyperlink ref="B6" r:id="rId5" display="iicecream@example.com"/>
     <hyperlink ref="B7" r:id="rId6" display="jjackfruit@example.com"/>
+    <hyperlink ref="B8" r:id="rId7" display="kkiwi@example.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Handle user update form data
</commit_message>
<xml_diff>
--- a/tests/resources/mock_pi_form.xlsx
+++ b/tests/resources/mock_pi_form.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
   <si>
     <t xml:space="preserve">Timestamp</t>
   </si>
@@ -143,6 +143,18 @@
   </si>
   <si>
     <t xml:space="preserve">MMMM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rraspberry@example.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Randall</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raspberry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RRRR</t>
   </si>
 </sst>
 </file>
@@ -288,10 +300,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
+      <selection pane="bottomLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="1" style="0" width="21.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="30.02"/>
@@ -506,13 +518,27 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
+      <c r="A10" s="3" t="n">
+        <v>44105.3333333333</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="3"/>
@@ -604,6 +630,7 @@
     <hyperlink ref="B7" r:id="rId6" display="jjackfruit@example.com"/>
     <hyperlink ref="B8" r:id="rId7" display="kkiwi@example.com"/>
     <hyperlink ref="B9" r:id="rId8" display="mmango@example.com"/>
+    <hyperlink ref="B10" r:id="rId9" display="rraspberry@example.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Handle PI account cancellation
</commit_message>
<xml_diff>
--- a/tests/resources/mock_pi_form.xlsx
+++ b/tests/resources/mock_pi_form.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="49">
   <si>
     <t xml:space="preserve">Timestamp</t>
   </si>
@@ -155,6 +155,18 @@
   </si>
   <si>
     <t xml:space="preserve">RRRR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wwatermelon@example.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wanda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Watermelon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WWWW</t>
   </si>
 </sst>
 </file>
@@ -300,10 +312,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
+      <selection pane="bottomLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.58984375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.60546875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="1" style="0" width="21.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="30.02"/>
@@ -541,13 +553,27 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
+      <c r="A11" s="3" t="n">
+        <v>44185.3333333333</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="3"/>
@@ -631,6 +657,7 @@
     <hyperlink ref="B8" r:id="rId7" display="kkiwi@example.com"/>
     <hyperlink ref="B9" r:id="rId8" display="mmango@example.com"/>
     <hyperlink ref="B10" r:id="rId9" display="rraspberry@example.com"/>
+    <hyperlink ref="B11" r:id="rId10" display="wwatermelon@example.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>